<commit_message>
Update data sheets with missing logs
</commit_message>
<xml_diff>
--- a/04-Development-and-Quality-Assurance/Evaluation-Testing/Logs/Kali/Kali_Data.xlsx
+++ b/04-Development-and-Quality-Assurance/Evaluation-Testing/Logs/Kali/Kali_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://autuni-my.sharepoint.com/personal/cgr2690_autuni_ac_nz/Documents/Data/COMP703/Linux Networking/04-Development-and-Quality-Assurance/Logs/Kali/Run8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://autuni-my.sharepoint.com/personal/cgr2690_autuni_ac_nz/Documents/Data/COMP703/Linux Networking/04-Development-and-Quality-Assurance/Evaluation-Testing/Logs/Kali/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_1A0B8F4F527255435991DA6AD05ADE5EEEC8095E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73CFE85B-5EE4-43CD-83F9-EF9FF7600F06}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="11_1A0B8F4F527255435991DA6AD05ADE5EEEC8095E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A41112F3-AD76-4E73-8CB7-4BD845B0DE46}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="39">
   <si>
     <t>128</t>
   </si>
@@ -149,12 +149,18 @@
   <si>
     <t>IPv6 UDP</t>
   </si>
+  <si>
+    <t>IPv4</t>
+  </si>
+  <si>
+    <t>IPv6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,13 +168,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,11 +208,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,7 +314,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$3</c:f>
+              <c:f>Sheet1!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -320,7 +349,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -365,7 +394,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$15</c:f>
+              <c:f>Sheet1!$C$7:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -420,7 +449,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$3</c:f>
+              <c:f>Sheet1!$I$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -455,7 +484,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -500,7 +529,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$4:$I$15</c:f>
+              <c:f>Sheet1!$I$7:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -831,7 +860,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$3</c:f>
+              <c:f>Sheet1!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -866,7 +895,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -911,7 +940,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$15</c:f>
+              <c:f>Sheet1!$D$7:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -966,7 +995,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$3</c:f>
+              <c:f>Sheet1!$J$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1001,7 +1030,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1046,7 +1075,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$4:$J$15</c:f>
+              <c:f>Sheet1!$J$7:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1327,7 +1356,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>Average BitRate</a:t>
+              <a:t>Average Bitrate</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1372,7 +1401,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$3</c:f>
+              <c:f>Sheet1!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1407,7 +1436,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1452,7 +1481,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$15</c:f>
+              <c:f>Sheet1!$E$7:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1507,7 +1536,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$3</c:f>
+              <c:f>Sheet1!$K$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1542,7 +1571,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1587,7 +1616,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$4:$K$15</c:f>
+              <c:f>Sheet1!$K$7:$K$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1868,7 +1897,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>Average Packet Loss</a:t>
+              <a:t>Average Packetloss</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1913,7 +1942,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$3</c:f>
+              <c:f>Sheet1!$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1948,7 +1977,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1993,7 +2022,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$15</c:f>
+              <c:f>Sheet1!$F$7:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2048,7 +2077,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$3</c:f>
+              <c:f>Sheet1!$L$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2083,7 +2112,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$15</c:f>
+              <c:f>Sheet1!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2128,7 +2157,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$15</c:f>
+              <c:f>Sheet1!$L$7:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2461,7 +2490,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$3</c:f>
+              <c:f>Sheet1!$T$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2496,7 +2525,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2541,7 +2570,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$4:$T$15</c:f>
+              <c:f>Sheet1!$T$7:$T$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2596,7 +2625,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Z$3</c:f>
+              <c:f>Sheet1!$Z$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2631,7 +2660,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2676,7 +2705,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$4:$Z$15</c:f>
+              <c:f>Sheet1!$Z$7:$Z$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3009,7 +3038,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$3</c:f>
+              <c:f>Sheet1!$U$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3044,7 +3073,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3089,7 +3118,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$4:$U$15</c:f>
+              <c:f>Sheet1!$U$7:$U$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3144,7 +3173,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AA$3</c:f>
+              <c:f>Sheet1!$AA$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3179,7 +3208,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3224,7 +3253,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AA$4:$AA$15</c:f>
+              <c:f>Sheet1!$AA$7:$AA$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3512,7 +3541,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Average BitRate</a:t>
+              <a:t>Average Bitrate</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3557,7 +3586,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$3</c:f>
+              <c:f>Sheet1!$V$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3592,7 +3621,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3637,7 +3666,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$4:$V$15</c:f>
+              <c:f>Sheet1!$V$7:$V$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3692,7 +3721,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AB$3</c:f>
+              <c:f>Sheet1!$AB$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3727,7 +3756,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3772,7 +3801,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AB$4:$AB$15</c:f>
+              <c:f>Sheet1!$AB$7:$AB$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4060,7 +4089,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Average Packet Loss</a:t>
+              <a:t>Average Packetloss</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4105,7 +4134,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$W$3</c:f>
+              <c:f>Sheet1!$W$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4140,7 +4169,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4185,7 +4214,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$4:$W$15</c:f>
+              <c:f>Sheet1!$W$7:$W$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4240,7 +4269,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AC$3</c:f>
+              <c:f>Sheet1!$AC$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4275,7 +4304,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$15</c:f>
+              <c:f>Sheet1!$S$7:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4320,7 +4349,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AC$4:$AC$15</c:f>
+              <c:f>Sheet1!$AC$7:$AC$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -8915,15 +8944,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>588307</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>169209</xdr:rowOff>
+      <xdr:colOff>442630</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>12327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>319366</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>54909</xdr:rowOff>
+      <xdr:colOff>173689</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>88527</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8951,15 +8980,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>539483</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>155601</xdr:rowOff>
+      <xdr:colOff>393806</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>189219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>270543</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>41301</xdr:rowOff>
+      <xdr:colOff>124866</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>74919</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8987,15 +9016,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>397808</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>179613</xdr:rowOff>
+      <xdr:colOff>252131</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>22731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>128866</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>65313</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>588306</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>98931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9023,15 +9052,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>360189</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>168407</xdr:rowOff>
+      <xdr:colOff>214512</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>11525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>91248</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>54107</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>550688</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>87725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9058,16 +9087,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>588308</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>169209</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>16807</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>23532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>319367</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>54909</xdr:rowOff>
+      <xdr:colOff>352984</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>99732</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9094,16 +9123,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>587508</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>103576</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>16007</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>148399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>318566</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>179776</xdr:rowOff>
+      <xdr:colOff>352183</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>34099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9131,15 +9160,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>377796</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4322</xdr:rowOff>
+      <xdr:colOff>411413</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>49145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>108855</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>80522</xdr:rowOff>
+      <xdr:colOff>142472</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>125345</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9167,15 +9196,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>397008</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>108377</xdr:rowOff>
+      <xdr:colOff>430625</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>153200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>128067</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>184577</xdr:rowOff>
+      <xdr:colOff>161684</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>38900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9201,10 +9230,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9492,856 +9517,925 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241AF353-C3A0-40A6-A389-2EE7141C0FF3}">
-  <dimension ref="B2:AC15"/>
+  <dimension ref="B2:AG18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM25" sqref="AM25"/>
+      <selection activeCell="AO18" sqref="AO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="17" max="18" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="T2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+    </row>
+    <row r="5" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="S2" s="1" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="S5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="Y2" s="1" t="s">
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="Y5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-    </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I6" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J6" t="s">
         <v>30</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K6" t="s">
         <v>31</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L6" t="s">
         <v>32</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S6" t="s">
         <v>10</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T6" t="s">
         <v>25</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U6" t="s">
         <v>26</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V6" t="s">
         <v>27</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W6" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y6" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z6" t="s">
         <v>29</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA6" t="s">
         <v>30</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB6" t="s">
         <v>31</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>128</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>5.1900000000000004E-4</v>
       </c>
-      <c r="D4">
+      <c r="D7">
         <v>9.8499999999999995E-5</v>
       </c>
-      <c r="E4">
+      <c r="E7">
         <v>17245.820185099998</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>128</v>
       </c>
-      <c r="I4">
+      <c r="I7">
         <v>3.9450000000000005E-4</v>
       </c>
-      <c r="J4">
+      <c r="J7">
         <v>4.6299999999999994E-5</v>
       </c>
-      <c r="K4">
+      <c r="K7">
         <v>17456.933687000001</v>
       </c>
-      <c r="L4">
+      <c r="L7">
         <v>0.09</v>
       </c>
-      <c r="S4">
+      <c r="S7">
         <v>128</v>
       </c>
-      <c r="T4">
+      <c r="T7">
         <v>5.9690000000000003E-4</v>
       </c>
-      <c r="U4">
+      <c r="U7">
         <v>9.7E-5</v>
       </c>
-      <c r="V4">
+      <c r="V7">
         <v>17261.783222099999</v>
       </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
         <v>128</v>
       </c>
-      <c r="Z4">
+      <c r="Z7">
         <v>1.305E-4</v>
       </c>
-      <c r="AA4">
+      <c r="AA7">
         <v>4.6099999999999996E-5</v>
       </c>
-      <c r="AB4">
+      <c r="AB7">
         <v>17449.604368099997</v>
       </c>
-      <c r="AC4">
+      <c r="AC7">
         <v>5.2000000000000005E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>256</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>5.1509999999999989E-4</v>
       </c>
-      <c r="D5">
+      <c r="D8">
         <v>9.0400000000000015E-5</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>34804.3220115</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>256</v>
       </c>
-      <c r="I5">
+      <c r="I8">
         <v>4.3400000000000003E-4</v>
       </c>
-      <c r="J5">
+      <c r="J8">
         <v>4.7099999999999993E-5</v>
       </c>
-      <c r="K5">
+      <c r="K8">
         <v>34942.620202500002</v>
       </c>
-      <c r="L5">
+      <c r="L8">
         <v>6.0000000000000012E-2</v>
       </c>
-      <c r="S5">
+      <c r="S8">
         <v>256</v>
       </c>
-      <c r="T5">
+      <c r="T8">
         <v>5.5079999999999994E-4</v>
       </c>
-      <c r="U5">
+      <c r="U8">
         <v>9.0300000000000013E-5</v>
       </c>
-      <c r="V5">
+      <c r="V8">
         <v>34817.985176900009</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
         <v>256</v>
       </c>
-      <c r="Z5">
+      <c r="Z8">
         <v>1.651E-4</v>
       </c>
-      <c r="AA5">
+      <c r="AA8">
         <v>4.7000000000000004E-5</v>
       </c>
-      <c r="AB5">
+      <c r="AB8">
         <v>34920.658910500002</v>
       </c>
-      <c r="AC5">
+      <c r="AC8">
         <v>6.4000000000000015E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>384</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>8.8909999999999998E-4</v>
       </c>
-      <c r="D6">
+      <c r="D9">
         <v>8.7799999999999993E-5</v>
       </c>
-      <c r="E6">
+      <c r="E9">
         <v>52601.005454100006</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="H6">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>384</v>
       </c>
-      <c r="I6">
+      <c r="I9">
         <v>4.3939999999999995E-4</v>
       </c>
-      <c r="J6">
+      <c r="J9">
         <v>4.4600000000000007E-5</v>
       </c>
-      <c r="K6">
+      <c r="K9">
         <v>52154.577835999997</v>
       </c>
-      <c r="L6">
+      <c r="L9">
         <v>6.0000000000000012E-2</v>
       </c>
-      <c r="S6">
+      <c r="S9">
         <v>384</v>
       </c>
-      <c r="T6">
+      <c r="T9">
         <v>9.2360000000000012E-4</v>
       </c>
-      <c r="U6">
+      <c r="U9">
         <v>8.8299999999999978E-5</v>
       </c>
-      <c r="V6">
+      <c r="V9">
         <v>52553.033332400002</v>
       </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
         <v>384</v>
       </c>
-      <c r="Z6">
+      <c r="Z9">
         <v>1.9290000000000003E-4</v>
       </c>
-      <c r="AA6">
+      <c r="AA9">
         <v>4.4299999999999993E-5</v>
       </c>
-      <c r="AB6">
+      <c r="AB9">
         <v>52295.464183899996</v>
       </c>
-      <c r="AC6">
+      <c r="AC9">
         <v>5.6000000000000008E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>512</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>9.3680000000000011E-4</v>
       </c>
-      <c r="D7">
+      <c r="D10">
         <v>8.5400000000000016E-5</v>
       </c>
-      <c r="E7">
+      <c r="E10">
         <v>70083.514447100009</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="H7">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>512</v>
       </c>
-      <c r="I7">
+      <c r="I10">
         <v>4.1780000000000002E-4</v>
       </c>
-      <c r="J7">
+      <c r="J10">
         <v>3.4700000000000003E-5</v>
       </c>
-      <c r="K7">
+      <c r="K10">
         <v>69797.020971200007</v>
       </c>
-      <c r="L7">
+      <c r="L10">
         <v>0.10800000000000001</v>
       </c>
-      <c r="S7">
+      <c r="S10">
         <v>512</v>
       </c>
-      <c r="T7">
+      <c r="T10">
         <v>6.4900000000000005E-4</v>
       </c>
-      <c r="U7">
+      <c r="U10">
         <v>8.3399999999999994E-5</v>
       </c>
-      <c r="V7">
+      <c r="V10">
         <v>70126.190825999991</v>
       </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
         <v>512</v>
       </c>
-      <c r="Z7">
+      <c r="Z10">
         <v>1.9689999999999999E-4</v>
       </c>
-      <c r="AA7">
+      <c r="AA10">
         <v>3.4099999999999995E-5</v>
       </c>
-      <c r="AB7">
+      <c r="AB10">
         <v>69766.4187676</v>
       </c>
-      <c r="AC7">
+      <c r="AC10">
         <v>5.3000000000000005E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>640</v>
       </c>
-      <c r="C8">
+      <c r="C11">
         <v>1.0509E-3</v>
       </c>
-      <c r="D8">
+      <c r="D11">
         <v>8.6300000000000011E-5</v>
       </c>
-      <c r="E8">
+      <c r="E11">
         <v>87896.877479699993</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="H8">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>640</v>
       </c>
-      <c r="I8">
+      <c r="I11">
         <v>4.103E-4</v>
       </c>
-      <c r="J8">
+      <c r="J11">
         <v>2.5100000000000004E-5</v>
       </c>
-      <c r="K8">
+      <c r="K11">
         <v>86995.931843299986</v>
       </c>
-      <c r="L8">
+      <c r="L11">
         <v>5.2000000000000005E-2</v>
       </c>
-      <c r="S8">
+      <c r="S11">
         <v>640</v>
       </c>
-      <c r="T8">
+      <c r="T11">
         <v>8.3900000000000001E-4</v>
       </c>
-      <c r="U8">
+      <c r="U11">
         <v>8.5900000000000014E-5</v>
       </c>
-      <c r="V8">
+      <c r="V11">
         <v>88080.382773500009</v>
       </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
         <v>640</v>
       </c>
-      <c r="Z8">
+      <c r="Z11">
         <v>2.1990000000000001E-4</v>
       </c>
-      <c r="AA8">
+      <c r="AA11">
         <v>2.5600000000000006E-5</v>
       </c>
-      <c r="AB8">
+      <c r="AB11">
         <v>87305.134951700005</v>
       </c>
-      <c r="AC8">
+      <c r="AC11">
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>768</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>7.17309E-2</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <v>1.2000000000000002E-4</v>
       </c>
-      <c r="E9">
+      <c r="E12">
         <v>93581.590693999999</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>768</v>
       </c>
-      <c r="I9">
+      <c r="I12">
         <v>5.0905999999999989E-3</v>
       </c>
-      <c r="J9">
+      <c r="J12">
         <v>1.9699999999999999E-4</v>
       </c>
-      <c r="K9">
+      <c r="K12">
         <v>91091.661662600003</v>
       </c>
-      <c r="L9">
+      <c r="L12">
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="S9">
+      <c r="S12">
         <v>768</v>
       </c>
-      <c r="T9">
+      <c r="T12">
         <v>6.9628200000000001E-2</v>
       </c>
-      <c r="U9">
+      <c r="U12">
         <v>1.2000000000000002E-4</v>
       </c>
-      <c r="V9">
+      <c r="V12">
         <v>93563.075730600001</v>
       </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
         <v>768</v>
       </c>
-      <c r="Z9">
+      <c r="Z12">
         <v>4.9291999999999999E-3</v>
       </c>
-      <c r="AA9">
+      <c r="AA12">
         <v>2.0130000000000001E-4</v>
       </c>
-      <c r="AB9">
+      <c r="AB12">
         <v>91087.538745800004</v>
       </c>
-      <c r="AC9">
+      <c r="AC12">
         <v>6.0000000000000012E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B13">
         <v>896</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <v>7.6499400000000009E-2</v>
       </c>
-      <c r="D10">
+      <c r="D13">
         <v>1.4100000000000004E-4</v>
       </c>
-      <c r="E10">
+      <c r="E13">
         <v>93572.373676800009</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>896</v>
       </c>
-      <c r="I10">
+      <c r="I13">
         <v>5.8661999999999994E-3</v>
       </c>
-      <c r="J10">
+      <c r="J13">
         <v>3.9160000000000003E-4</v>
       </c>
-      <c r="K10">
+      <c r="K13">
         <v>92280.248612299998</v>
       </c>
-      <c r="L10">
+      <c r="L13">
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="S10">
+      <c r="S13">
         <v>896</v>
       </c>
-      <c r="T10">
+      <c r="T13">
         <v>7.6671800000000012E-2</v>
       </c>
-      <c r="U10">
+      <c r="U13">
         <v>1.4090000000000004E-4</v>
       </c>
-      <c r="V10">
+      <c r="V13">
         <v>93584.696719300002</v>
       </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
         <v>896</v>
       </c>
-      <c r="Z10">
+      <c r="Z13">
         <v>5.7063000000000001E-3</v>
       </c>
-      <c r="AA10">
+      <c r="AA13">
         <v>3.9110000000000002E-4</v>
       </c>
-      <c r="AB10">
+      <c r="AB13">
         <v>92320.009301600003</v>
       </c>
-      <c r="AC10">
+      <c r="AC13">
         <v>4.9999999999999996E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>1024</v>
       </c>
-      <c r="C11">
+      <c r="C14">
         <v>7.5401599999999999E-2</v>
       </c>
-      <c r="D11">
+      <c r="D14">
         <v>1.6150000000000002E-4</v>
       </c>
-      <c r="E11">
+      <c r="E14">
         <v>93631.19045899999</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="H11">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>1024</v>
       </c>
-      <c r="I11">
+      <c r="I14">
         <v>6.5946000000000008E-3</v>
       </c>
-      <c r="J11">
+      <c r="J14">
         <v>5.6949999999999991E-4</v>
       </c>
-      <c r="K11">
+      <c r="K14">
         <v>93294.213047600002</v>
       </c>
-      <c r="L11">
+      <c r="L14">
         <v>4.6999999999999993E-2</v>
       </c>
-      <c r="S11">
+      <c r="S14">
         <v>1024</v>
       </c>
-      <c r="T11">
+      <c r="T14">
         <v>7.7855099999999997E-2</v>
       </c>
-      <c r="U11">
+      <c r="U14">
         <v>1.6160000000000002E-4</v>
       </c>
-      <c r="V11">
+      <c r="V14">
         <v>93629.4816096</v>
       </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
         <v>1024</v>
       </c>
-      <c r="Z11">
+      <c r="Z14">
         <v>6.4381000000000004E-3</v>
       </c>
-      <c r="AA11">
+      <c r="AA14">
         <v>5.689E-4</v>
       </c>
-      <c r="AB11">
+      <c r="AB14">
         <v>93239.203584000003</v>
       </c>
-      <c r="AC11">
+      <c r="AC14">
         <v>9.2999999999999985E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>1152</v>
       </c>
-      <c r="C12">
+      <c r="C15">
         <v>7.8402199999999991E-2</v>
       </c>
-      <c r="D12">
+      <c r="D15">
         <v>1.8190000000000003E-4</v>
       </c>
-      <c r="E12">
+      <c r="E15">
         <v>93644.150759299999</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="H12">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>1152</v>
       </c>
-      <c r="I12">
+      <c r="I15">
         <v>7.3479999999999986E-3</v>
       </c>
-      <c r="J12">
+      <c r="J15">
         <v>7.1880000000000002E-4</v>
       </c>
-      <c r="K12">
+      <c r="K15">
         <v>93997.232500200029</v>
       </c>
-      <c r="L12">
+      <c r="L15">
         <v>8.299999999999999E-2</v>
       </c>
-      <c r="S12">
+      <c r="S15">
         <v>1152</v>
       </c>
-      <c r="T12">
+      <c r="T15">
         <v>7.5410699999999983E-2</v>
       </c>
-      <c r="U12">
+      <c r="U15">
         <v>1.8220000000000001E-4</v>
       </c>
-      <c r="V12">
+      <c r="V15">
         <v>93652.038279800006</v>
       </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
         <v>1152</v>
       </c>
-      <c r="Z12">
+      <c r="Z15">
         <v>7.2344999999999996E-3</v>
       </c>
-      <c r="AA12">
+      <c r="AA15">
         <v>7.2959999999999995E-4</v>
       </c>
-      <c r="AB12">
+      <c r="AB15">
         <v>94018.391845100006</v>
       </c>
-      <c r="AC12">
+      <c r="AC15">
         <v>5.2000000000000005E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B16">
         <v>1280</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>7.4444800000000005E-2</v>
       </c>
-      <c r="D13">
+      <c r="D16">
         <v>2.0259999999999999E-4</v>
       </c>
-      <c r="E13">
+      <c r="E16">
         <v>93654.461065800002</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>1280</v>
       </c>
-      <c r="I13">
+      <c r="I16">
         <v>8.3416000000000011E-3</v>
       </c>
-      <c r="J13">
+      <c r="J16">
         <v>8.5459999999999996E-4</v>
       </c>
-      <c r="K13">
+      <c r="K16">
         <v>94659.673357399995</v>
       </c>
-      <c r="L13">
+      <c r="L16">
         <v>1.8999999999999996E-2</v>
       </c>
-      <c r="S13">
+      <c r="S16">
         <v>1280</v>
       </c>
-      <c r="T13">
+      <c r="T16">
         <v>7.4295299999999995E-2</v>
       </c>
-      <c r="U13">
+      <c r="U16">
         <v>2.0250000000000004E-4</v>
       </c>
-      <c r="V13">
+      <c r="V16">
         <v>93688.74889979999</v>
       </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
         <v>1280</v>
       </c>
-      <c r="Z13">
+      <c r="Z16">
         <v>8.2635E-3</v>
       </c>
-      <c r="AA13">
+      <c r="AA16">
         <v>8.7139999999999993E-4</v>
       </c>
-      <c r="AB13">
+      <c r="AB16">
         <v>94569.700130700017</v>
       </c>
-      <c r="AC13">
+      <c r="AC16">
         <v>3.7999999999999992E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B17">
         <v>1408</v>
       </c>
-      <c r="C14">
+      <c r="C17">
         <v>7.5332099999999999E-2</v>
       </c>
-      <c r="D14">
+      <c r="D17">
         <v>2.2369999999999999E-4</v>
       </c>
-      <c r="E14">
+      <c r="E17">
         <v>93704.911762599993</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="H14">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>1408</v>
       </c>
-      <c r="I14">
+      <c r="I17">
         <v>9.0388000000000013E-3</v>
       </c>
-      <c r="J14">
+      <c r="J17">
         <v>9.9430000000000004E-4</v>
       </c>
-      <c r="K14">
+      <c r="K17">
         <v>95043.688907499993</v>
       </c>
-      <c r="L14">
+      <c r="L17">
         <v>0.217</v>
       </c>
-      <c r="S14">
+      <c r="S17">
         <v>1408</v>
       </c>
-      <c r="T14">
+      <c r="T17">
         <v>8.1909099999999999E-2</v>
       </c>
-      <c r="U14">
+      <c r="U17">
         <v>2.2359999999999996E-4</v>
       </c>
-      <c r="V14">
+      <c r="V17">
         <v>93685.618883300005</v>
       </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
         <v>1408</v>
       </c>
-      <c r="Z14">
+      <c r="Z17">
         <v>8.9073999999999993E-3</v>
       </c>
-      <c r="AA14">
+      <c r="AA17">
         <v>9.9170000000000009E-4</v>
       </c>
-      <c r="AB14">
+      <c r="AB17">
         <v>95105.498003800021</v>
       </c>
-      <c r="AC14">
+      <c r="AC17">
         <v>0.14499999999999996</v>
       </c>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B15">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B18">
         <v>1536</v>
       </c>
-      <c r="C15">
+      <c r="C18">
         <v>6.8223999999999993E-2</v>
       </c>
-      <c r="D15">
+      <c r="D18">
         <v>2.4439999999999998E-4</v>
       </c>
-      <c r="E15">
+      <c r="E18">
         <v>93745.519585699978</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>1536</v>
       </c>
-      <c r="I15">
+      <c r="I18">
         <v>7.3020000000000003E-3</v>
       </c>
-      <c r="J15">
+      <c r="J18">
         <v>9.1159999999999993E-4</v>
       </c>
-      <c r="K15">
+      <c r="K18">
         <v>91834.754220799994</v>
       </c>
-      <c r="L15">
+      <c r="L18">
         <v>2.9000000000000005E-2</v>
       </c>
-      <c r="S15">
+      <c r="S18">
         <v>1536</v>
       </c>
-      <c r="T15">
+      <c r="T18">
         <v>5.9132300000000006E-2</v>
       </c>
-      <c r="U15">
+      <c r="U18">
         <v>2.4380000000000002E-4</v>
       </c>
-      <c r="V15">
+      <c r="V18">
         <v>93837.239220600008</v>
       </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
         <v>1536</v>
       </c>
-      <c r="Z15">
+      <c r="Z18">
         <v>7.2446000000000012E-3</v>
       </c>
-      <c r="AA15">
+      <c r="AA18">
         <v>9.029000000000001E-4</v>
       </c>
-      <c r="AB15">
+      <c r="AB18">
         <v>91842.884035600015</v>
       </c>
-      <c r="AC15">
+      <c r="AC18">
         <v>3.2999999999999995E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="S2:W2"/>
-    <mergeCell ref="Y2:AC2"/>
+  <mergeCells count="6">
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="T2:AG3"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="S5:W5"/>
+    <mergeCell ref="Y5:AC5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>